<commit_message>
Finally merging with Fake hand sensor type
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sami\Desktop\SRT\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E713659-B810-4054-BE35-A7501B0D26DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F8D975-60C7-49C3-B0E0-D19D4FFAB7B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7BC8ADB8-7BDC-42AB-9E57-C69A6D9EC071}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -551,15 +550,15 @@
       </c>
       <c r="H2" t="str">
         <f t="shared" ref="H2:H27" ca="1" si="0">IF(RAND()&gt;0.5,"On","Off")</f>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="I2" t="str">
         <f t="shared" ref="I2:T17" ca="1" si="1">IF(RAND()&gt;0.5,"On","Off")</f>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="J2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="K2" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -567,11 +566,11 @@
       </c>
       <c r="L2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="M2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="N2" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -587,7 +586,7 @@
       </c>
       <c r="Q2" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="R2" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -599,17 +598,17 @@
       </c>
       <c r="T2" t="str">
         <f ca="1">IF(RAND()&gt;0.5,"On","Off")</f>
-        <v>Off</v>
+        <v>On</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -633,7 +632,7 @@
       </c>
       <c r="O3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="P3" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -641,11 +640,11 @@
       </c>
       <c r="Q3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="R3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="S3" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -653,21 +652,21 @@
       </c>
       <c r="T3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -683,7 +682,7 @@
       </c>
       <c r="N4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="O4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -691,19 +690,19 @@
       </c>
       <c r="P4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="Q4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="R4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="S4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="T4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -721,7 +720,7 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -741,7 +740,7 @@
       </c>
       <c r="O5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -749,7 +748,7 @@
       </c>
       <c r="Q5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="R5" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -771,7 +770,7 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -787,11 +786,11 @@
       </c>
       <c r="M6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -803,15 +802,15 @@
       </c>
       <c r="Q6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="R6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="S6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="T6" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -821,7 +820,7 @@
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -829,7 +828,7 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -841,19 +840,19 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="O7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="P7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -875,7 +874,7 @@
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -883,7 +882,7 @@
       </c>
       <c r="J8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -895,11 +894,11 @@
       </c>
       <c r="M8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -915,15 +914,15 @@
       </c>
       <c r="R8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="S8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="T8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -937,7 +936,7 @@
       </c>
       <c r="J9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -945,23 +944,23 @@
       </c>
       <c r="L9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="P9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="Q9" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -969,29 +968,29 @@
       </c>
       <c r="R9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="S9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="T9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -999,31 +998,31 @@
       </c>
       <c r="L10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="P10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="Q10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="R10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="S10" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1031,13 +1030,13 @@
       </c>
       <c r="T10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1049,7 +1048,7 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1057,7 +1056,7 @@
       </c>
       <c r="M11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1085,7 +1084,7 @@
       </c>
       <c r="T11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
@@ -1107,15 +1106,15 @@
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1123,15 +1122,15 @@
       </c>
       <c r="P12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="Q12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="S12" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1149,15 +1148,15 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1185,11 +1184,11 @@
       </c>
       <c r="R13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="S13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="T13" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1207,7 +1206,7 @@
       </c>
       <c r="J14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1223,11 +1222,11 @@
       </c>
       <c r="N14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="O14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="P14" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1239,11 +1238,11 @@
       </c>
       <c r="R14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="S14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="T14" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1261,7 +1260,7 @@
       </c>
       <c r="J15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1269,7 +1268,7 @@
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1277,15 +1276,15 @@
       </c>
       <c r="N15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="O15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="P15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1307,15 +1306,15 @@
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1331,31 +1330,31 @@
       </c>
       <c r="N16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="O16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="Q16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="T16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
     </row>
     <row r="17" spans="8:20" x14ac:dyDescent="0.3">
@@ -1365,11 +1364,11 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1385,11 +1384,11 @@
       </c>
       <c r="N17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="P17" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1397,11 +1396,11 @@
       </c>
       <c r="Q17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="R17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1415,15 +1414,15 @@
     <row r="18" spans="8:20" x14ac:dyDescent="0.3">
       <c r="H18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" ref="I18:T27" ca="1" si="2">IF(RAND()&gt;0.5,"On","Off")</f>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1455,7 +1454,7 @@
       </c>
       <c r="R18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="S18" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1473,7 +1472,7 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1489,11 +1488,11 @@
       </c>
       <c r="M19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="N19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="O19" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1513,7 +1512,7 @@
       </c>
       <c r="S19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="T19" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1523,7 +1522,7 @@
     <row r="20" spans="8:20" x14ac:dyDescent="0.3">
       <c r="H20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1559,7 +1558,7 @@
       </c>
       <c r="Q20" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="R20" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1571,13 +1570,13 @@
       </c>
       <c r="T20" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
     </row>
     <row r="21" spans="8:20" x14ac:dyDescent="0.3">
       <c r="H21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1585,19 +1584,19 @@
       </c>
       <c r="J21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1605,7 +1604,7 @@
       </c>
       <c r="O21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1613,7 +1612,7 @@
       </c>
       <c r="Q21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="R21" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1621,25 +1620,25 @@
       </c>
       <c r="S21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="T21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
     </row>
     <row r="22" spans="8:20" x14ac:dyDescent="0.3">
       <c r="H22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1659,27 +1658,27 @@
       </c>
       <c r="O22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="P22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="Q22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="R22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="S22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="T22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
     </row>
     <row r="23" spans="8:20" x14ac:dyDescent="0.3">
@@ -1689,7 +1688,7 @@
       </c>
       <c r="I23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1697,15 +1696,15 @@
       </c>
       <c r="K23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1713,7 +1712,7 @@
       </c>
       <c r="O23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="P23" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1721,15 +1720,15 @@
       </c>
       <c r="Q23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="R23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="S23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="T23" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1739,11 +1738,11 @@
     <row r="24" spans="8:20" x14ac:dyDescent="0.3">
       <c r="H24" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1759,7 +1758,7 @@
       </c>
       <c r="M24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1775,11 +1774,11 @@
       </c>
       <c r="Q24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="R24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="S24" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1787,7 +1786,7 @@
       </c>
       <c r="T24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
     </row>
     <row r="25" spans="8:20" x14ac:dyDescent="0.3">
@@ -1797,15 +1796,15 @@
       </c>
       <c r="I25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1821,7 +1820,7 @@
       </c>
       <c r="O25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="P25" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1829,7 +1828,7 @@
       </c>
       <c r="Q25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="R25" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1837,7 +1836,7 @@
       </c>
       <c r="S25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="T25" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1847,7 +1846,7 @@
     <row r="26" spans="8:20" x14ac:dyDescent="0.3">
       <c r="H26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1855,15 +1854,15 @@
       </c>
       <c r="J26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1875,11 +1874,11 @@
       </c>
       <c r="O26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="Q26" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1887,7 +1886,7 @@
       </c>
       <c r="R26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="S26" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1895,21 +1894,21 @@
       </c>
       <c r="T26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
     </row>
     <row r="27" spans="8:20" x14ac:dyDescent="0.3">
       <c r="H27" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1917,19 +1916,19 @@
       </c>
       <c r="L27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Off</v>
+        <v>On</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="P27" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1941,7 +1940,7 @@
       </c>
       <c r="R27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
       <c r="S27" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1949,7 +1948,7 @@
       </c>
       <c r="T27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>On</v>
+        <v>Off</v>
       </c>
     </row>
   </sheetData>

</xml_diff>